<commit_message>
fix the tableur parralax background endled into the boat
</commit_message>
<xml_diff>
--- a/texte.xlsx
+++ b/texte.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BB7B3E-6A1B-45A0-A138-8A5D8C3B428D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40848435-4D92-4E47-AFBD-0FB5DECE9E28}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54615" yWindow="435" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,23 +620,23 @@
         <v>416</v>
       </c>
       <c r="H2">
-        <f>F2-D2</f>
-        <v>239</v>
+        <f>D2-F2</f>
+        <v>-239</v>
       </c>
       <c r="I2">
-        <f>G2-E2</f>
-        <v>84</v>
+        <f>E2-G2</f>
+        <v>-84</v>
       </c>
       <c r="J2">
         <v>0.8</v>
       </c>
       <c r="K2">
-        <f>H2-(D2*J2)</f>
-        <v>161.39999999999998</v>
+        <f>H2+(F2*J2)</f>
+        <v>29.800000000000011</v>
       </c>
       <c r="L2">
-        <f>I2+(J2*E2)</f>
-        <v>349.6</v>
+        <f>I2+(J2*G2)</f>
+        <v>248.8</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
figur it out git status!
</commit_message>
<xml_diff>
--- a/texte.xlsx
+++ b/texte.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40848435-4D92-4E47-AFBD-0FB5DECE9E28}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CCBCC5-D1DD-4E4E-B9CF-E36DAFD76AD4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54615" yWindow="435" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>intro :</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>y_b</t>
+  </si>
+  <si>
+    <t>x_c</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -551,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L89"/>
+  <dimension ref="A1:R89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +568,7 @@
     <col min="3" max="3" width="99.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -590,14 +596,23 @@
       <c r="J1" t="s">
         <v>55</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>56</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -630,16 +645,27 @@
       <c r="J2">
         <v>0.8</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <f>H2+(F2*J2)</f>
         <v>29.800000000000011</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <f>I2+(J2*G2)</f>
         <v>248.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>0.5</v>
+      </c>
+      <c r="Q2">
+        <f>H2+(F2*O2)</f>
+        <v>-71</v>
+      </c>
+      <c r="R2">
+        <f>I2+(O2*G2)</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -647,7 +673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -655,7 +681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -663,7 +689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -671,7 +697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
@@ -679,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
@@ -687,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
@@ -695,7 +721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
@@ -703,7 +729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
@@ -711,12 +737,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>11</v>
       </c>
@@ -724,7 +750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>12</v>
       </c>
@@ -732,7 +758,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>13</v>
       </c>
@@ -740,7 +766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>14</v>
       </c>

</xml_diff>